<commit_message>
Entered Sept 2025 COMPASS Syn Sulfide Data
</commit_message>
<xml_diff>
--- a/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/COMPASS_Sept2025_Plate6+7_20250925.xlsx
+++ b/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/COMPASS_Sept2025_Plate6+7_20250925.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20346"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\microplate\Desktop\BioGeoChem_Microplates\COMPASS\H2S\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sinet-my.sharepoint.com/personal/readz_si_edu1/Documents/synoptic-discrete-data/Porewater/Sulfide/Synoptic_CB/2025/September/Raw Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DF5B22D-FCE9-4907-A23C-574D05B8D12B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{2DF5B22D-FCE9-4907-A23C-574D05B8D12B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A42DAD5B-B857-428D-AAAB-754B91B052B9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18885" windowHeight="11640" xr2:uid="{0B0B4313-D15F-4D56-B951-581B53B7BFD4}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" xr2:uid="{0B0B4313-D15F-4D56-B951-581B53B7BFD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1145,9 +1156,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1185,7 +1196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1291,7 +1302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1433,7 +1444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1444,12 +1455,12 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -1488,7 +1499,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1532,7 +1543,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1576,7 +1587,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1620,7 +1631,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -1664,7 +1675,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1752,7 +1763,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1799,7 +1810,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1846,7 +1857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1867,7 +1878,7 @@
         <v>0.60433333333333328</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1888,7 +1899,7 @@
         <v>0.66233333333333333</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12.5</v>
       </c>
@@ -1909,7 +1920,7 @@
         <v>0.50800000000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>25</v>
       </c>
@@ -1930,7 +1941,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>50</v>
       </c>
@@ -1951,7 +1962,7 @@
         <v>2.7530000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>100</v>
       </c>
@@ -1972,7 +1983,7 @@
         <v>0.12933333333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>1.1293333333333333</v>
@@ -1990,7 +2001,7 @@
         <v>7.4666666666666659E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>1.2150000000000001</v>
@@ -2008,7 +2019,7 @@
         <v>4.5000000000000005E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="2">
         <v>1</v>
@@ -2047,7 +2058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>0</v>
       </c>
@@ -2091,7 +2102,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>1</v>
       </c>
@@ -2135,7 +2146,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
@@ -2179,7 +2190,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>3</v>
       </c>
@@ -2223,7 +2234,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>4</v>
       </c>
@@ -2267,7 +2278,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -2311,7 +2322,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -2358,7 +2369,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>